<commit_message>
modify for tcc ipc
</commit_message>
<xml_diff>
--- a/Linux/DeviceDrivers/Document(important)/02.并发与竞态.xlsx
+++ b/Linux/DeviceDrivers/Document(important)/02.并发与竞态.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C562BB72-F14F-4267-92CE-2A4E79FBD12E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76926CB0-48BC-48CD-9B69-273058FE79CB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="845" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="atomic_hc" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="mutex_hc" sheetId="7" r:id="rId9"/>
     <sheet name="mutex_sam" sheetId="14" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1495,8 +1495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E42"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -2908,7 +2908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:E78"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C40" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
@@ -3452,7 +3452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:E37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>

</xml_diff>